<commit_message>
Se agrego extensiones para Reec.Helpers para su proxima versión.
</commit_message>
<xml_diff>
--- a/documents/Documentacion de error.xlsx
+++ b/documents/Documentacion de error.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edy\source\repos\Reec\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F0478E-D38C-4EE2-98EC-602191DEB8FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A9E4FA-64BA-4F63-AD83-78AE4FF1CCF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1026,7 +1026,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -1358,7 +1358,7 @@
   <dimension ref="A2:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1545,7 +1545,7 @@
         <v>502</v>
       </c>
       <c r="C13" s="4">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>109</v>
@@ -1561,7 +1561,7 @@
         <v>504</v>
       </c>
       <c r="C14" s="4">
-        <v>500</v>
+        <v>504</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>110</v>

</xml_diff>